<commit_message>
Changes in README, Validation, Test-Preferences
</commit_message>
<xml_diff>
--- a/Notebooks/Test-Data.xlsx
+++ b/Notebooks/Test-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/missd/Desktop/ML2 - Abschlussprojekt/ml2_project/Notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC34A88-15A7-2845-8039-43199A411843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D41A08-BD45-3B4A-96D4-114F2F00BBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="-20700" windowWidth="30620" windowHeight="17100" xr2:uid="{0ABD31C3-C47E-024F-8978-93A71FAD6E05}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t>AktivTeilnehmen</t>
   </si>
@@ -83,9 +83,6 @@
     <t>noch nicht</t>
   </si>
   <si>
-    <t>Durch die Mediaktion ist eine deutliche Verbesserung betreffend seiner Aufmerksamkeitsspanne und Impulsregulation erkennbar.</t>
-  </si>
-  <si>
     <t>Man merkt, dass er zwar gute Leistungen erbringen möchte, für diese aber möglichst wenig Aufwand betreiben möchte.</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>Firstname</t>
   </si>
   <si>
-    <t>John01 ist im Unterricht meist aktiv dabei. Insbesondere bei Fächern, welche ihn interessieren. Durch die Mediaktion ist eine deutliche Verbesserung betreffend seiner Aufmerksamkeitsspanne und Impulsregulation erkennbar, so dass er im Unterricht gute Leistungen zeigen kann. Es gelingt ihm meist, aufmerksam zu sein und den Instruktionen der Lehrperson zu folgen. John01 merkt sich die meisten Schulinhalte, vergisst sie jedoch, sobald das Thema abgeschlossen wird. So kann das Wissen später kaum abgerufen werden. Man merkt zwar, dass er gute Leistungen erbringen möchte, er ist aber noch nicht bereit, für diese auch Aufwand zu betreiben.</t>
-  </si>
-  <si>
     <t xml:space="preserve">John02 ist im Unterricht meist aktiv dabei. Insbesondere bei Fächern, welche ihn interessieren. Er zeigt generell gute Leistungen im Unterricht. Es gelingt ihm meist, aufmerksam zu sein und den Instruktionen der Lehrperson zu folgen. John02 merkt sich die meisten Schulinhalte, vergisst sie jedoch, sobald das Thema abgeschlossen wird. So kann das Wissen später kaum abgerufen werden. </t>
   </si>
   <si>
@@ -207,6 +201,12 @@
   </si>
   <si>
     <t xml:space="preserve">John10 ist im Unterricht oftmals sehr bemüht, aktiv mitzumachen. Es kommt regelmässig vor, dass er sich durch unangenehme Situationen in seinem Privatleben oder durch soziale Konflikte nicht auf den Unterrichtsstoff einlassen kann. Es gelingt ihm auch noch nicht immer, aufmerksam zu sein und den Instruktionen der Lehrperson zu folgen. Es sind aber deutliche Fortschritte erkennbar. John10 kann sich Schulinhalte immer besser merken und sie bei Bedarf abrufen. </t>
+  </si>
+  <si>
+    <t>Durch die Medikation ist eine deutliche Verbesserung betreffend seiner Aufmerksamkeitsspanne und Impulsregulation erkennbar.</t>
+  </si>
+  <si>
+    <t>John01 ist im Unterricht meist aktiv dabei. Insbesondere bei Fächern, welche ihn interessieren. Durch die Medikation ist eine deutliche Verbesserung betreffend seiner Aufmerksamkeitsspanne und Impulsregulation erkennbar, so dass er im Unterricht gute Leistungen zeigen kann. Es gelingt ihm meist, aufmerksam zu sein und den Instruktionen der Lehrperson zu folgen. John01 merkt sich die meisten Schulinhalte, vergisst sie jedoch, sobald das Thema abgeschlossen wird. So kann das Wissen später kaum abgerufen werden. Man merkt zwar, dass er gute Leistungen erbringen möchte, er ist aber noch nicht bereit, für diese auch Aufwand zu betreiben.</t>
   </si>
 </sst>
 </file>
@@ -862,7 +862,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,7 +875,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -908,18 +908,18 @@
         <v>9</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="153" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>10</v>
@@ -933,19 +933,19 @@
         <v>12</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="13"/>
       <c r="L2" s="6" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>10</v>
@@ -968,12 +968,12 @@
       </c>
       <c r="K3" s="15"/>
       <c r="L3" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="221" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>10</v>
@@ -983,7 +983,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>10</v>
@@ -997,15 +997,15 @@
         <v>13</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>10</v>
@@ -1028,30 +1028,30 @@
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>10</v>
@@ -1062,18 +1062,18 @@
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="289" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>14</v>
@@ -1083,25 +1083,25 @@
         <v>12</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="15"/>
       <c r="L7" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="372" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>13</v>
@@ -1115,25 +1115,25 @@
         <v>12</v>
       </c>
       <c r="G8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>12</v>
@@ -1143,7 +1143,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>10</v>
@@ -1153,21 +1153,21 @@
         <v>10</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>10</v>
@@ -1185,52 +1185,52 @@
         <v>10</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="K10" s="15"/>
       <c r="L10" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="205" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="17" t="s">
+      <c r="J11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>31</v>
-      </c>
       <c r="L11" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>